<commit_message>
Timing diagram and block diagram 1st version
</commit_message>
<xml_diff>
--- a/timing-diagram/timing_analysis_data.xlsx
+++ b/timing-diagram/timing_analysis_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AME_Block-Diagram\timing-diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CFC1DB-45BA-4348-8F8A-A65DAFEC1A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC440D53-0741-43ED-943A-7458EE937EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B0B85157-5F58-4FAA-AB16-990C0694D044}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>w</t>
   </si>
@@ -64,7 +64,19 @@
     <t>2*</t>
   </si>
   <si>
-    <t>Considering that the Affine ME process is just the 17% of the ME complexity</t>
+    <t>Clock Cycles required (16x16 extimation)</t>
+  </si>
+  <si>
+    <t>Percentage of the total comp. Complexity</t>
+  </si>
+  <si>
+    <t>Percentage of the ME complexity</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Considering also that the Affine ME process is just the 17% of the ME complexity</t>
   </si>
 </sst>
 </file>
@@ -124,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -136,21 +148,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -161,17 +158,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -188,15 +174,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -217,17 +194,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -305,31 +271,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -644,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBD2D36-072C-4FA3-BFF3-6C9E50610318}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,373 +620,397 @@
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2560</v>
       </c>
       <c r="B2" s="2">
         <v>1600</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>30</v>
       </c>
-      <c r="D2" s="10">
-        <f>(((A2*B2)/256)*50*C2)/(10^6)</f>
+      <c r="D2" s="1">
+        <f>(((A2*B2)/256)*$K$4*C2)/(10^6)</f>
+        <v>24.48</v>
+      </c>
+      <c r="E2" s="17">
+        <f>D2*(100/$K$6)</f>
+        <v>46.188679245283019</v>
+      </c>
+      <c r="F2" s="7">
+        <f>E2*(100/$K$8)</f>
+        <v>271.69811320754718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1920</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1080</v>
+      </c>
+      <c r="C3" s="4">
+        <v>60</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D16" si="0">(((A3*B3)/256)*$K$4*C3)/(10^6)</f>
+        <v>24.786000000000001</v>
+      </c>
+      <c r="E3" s="18">
+        <f t="shared" ref="E3:E16" si="1">D3*(100/$K$6)</f>
+        <v>46.766037735849061</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F16" si="2">E3*(100/$K$8)</f>
+        <v>275.09433962264154</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1920</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1080</v>
+      </c>
+      <c r="C4" s="4">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>20.655000000000001</v>
+      </c>
+      <c r="E4" s="18">
+        <f t="shared" si="1"/>
+        <v>38.971698113207552</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="2"/>
+        <v>229.24528301886798</v>
+      </c>
+      <c r="K4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1920</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1080</v>
+      </c>
+      <c r="C5" s="4">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>12.393000000000001</v>
+      </c>
+      <c r="E5" s="18">
+        <f t="shared" si="1"/>
+        <v>23.38301886792453</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="2"/>
+        <v>137.54716981132077</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1920</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1080</v>
+      </c>
+      <c r="C6" s="4">
         <v>24</v>
       </c>
-      <c r="E2" s="13">
-        <f>D2*(100/53)</f>
-        <v>45.283018867924525</v>
-      </c>
-      <c r="F2" s="13">
-        <f>E2*(100/17)</f>
-        <v>266.37069922308547</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1920</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1080</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>9.9144000000000005</v>
+      </c>
+      <c r="E6" s="18">
+        <f t="shared" si="1"/>
+        <v>18.706415094339626</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="2"/>
+        <v>110.03773584905663</v>
+      </c>
+      <c r="K6">
+        <v>53</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1280</v>
+      </c>
+      <c r="B7" s="4">
+        <v>720</v>
+      </c>
+      <c r="C7" s="4">
         <v>60</v>
       </c>
-      <c r="D3" s="11">
-        <f>(((A3*B3)/256)*50*C3)/(10^6)</f>
-        <v>24.3</v>
-      </c>
-      <c r="E3" s="14">
-        <f t="shared" ref="E3:E16" si="0">D3*(100/53)</f>
-        <v>45.84905660377359</v>
-      </c>
-      <c r="F3" s="14">
-        <f t="shared" ref="F3:F16" si="1">E3*(100/17)</f>
-        <v>269.70033296337408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1920</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1080</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>11.016</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" si="1"/>
+        <v>20.784905660377358</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="2"/>
+        <v>122.26415094339623</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1280</v>
+      </c>
+      <c r="B8" s="4">
+        <v>720</v>
+      </c>
+      <c r="C8" s="4">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>5.508</v>
+      </c>
+      <c r="E8" s="18">
+        <f t="shared" si="1"/>
+        <v>10.392452830188679</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="2"/>
+        <v>61.132075471698116</v>
+      </c>
+      <c r="K8">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1280</v>
+      </c>
+      <c r="B9" s="4">
+        <v>720</v>
+      </c>
+      <c r="C9" s="4">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>3.6720000000000002</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" si="1"/>
+        <v>6.9283018867924531</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="2"/>
+        <v>40.754716981132077</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1024</v>
+      </c>
+      <c r="B10" s="4">
+        <v>768</v>
+      </c>
+      <c r="C10" s="4">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>4.7001600000000003</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" si="1"/>
+        <v>8.8682264150943411</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="2"/>
+        <v>52.166037735849066</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>832</v>
+      </c>
+      <c r="B11" s="4">
+        <v>480</v>
+      </c>
+      <c r="C11" s="4">
+        <v>60</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>4.7736000000000001</v>
+      </c>
+      <c r="E11" s="18">
+        <f t="shared" si="1"/>
+        <v>9.0067924528301884</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="2"/>
+        <v>52.981132075471699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>832</v>
+      </c>
+      <c r="B12" s="4">
+        <v>480</v>
+      </c>
+      <c r="C12" s="4">
         <v>50</v>
       </c>
-      <c r="D4" s="11">
-        <f>(((A4*B4)/256)*50*C4)/(10^6)</f>
-        <v>20.25</v>
-      </c>
-      <c r="E4" s="14">
-        <f t="shared" si="0"/>
-        <v>38.20754716981132</v>
-      </c>
-      <c r="F4" s="14">
-        <f t="shared" si="1"/>
-        <v>224.75027746947836</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1920</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1080</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>3.9780000000000002</v>
+      </c>
+      <c r="E12" s="18">
+        <f t="shared" si="1"/>
+        <v>7.5056603773584909</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="2"/>
+        <v>44.150943396226417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>832</v>
+      </c>
+      <c r="B13" s="4">
+        <v>480</v>
+      </c>
+      <c r="C13" s="4">
         <v>30</v>
       </c>
-      <c r="D5" s="11">
-        <f>(((A5*B5)/256)*50*C5)/(10^6)</f>
-        <v>12.15</v>
-      </c>
-      <c r="E5" s="14">
-        <f t="shared" si="0"/>
-        <v>22.924528301886795</v>
-      </c>
-      <c r="F5" s="14">
-        <f t="shared" si="1"/>
-        <v>134.85016648168704</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1920</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1080</v>
-      </c>
-      <c r="C6" s="6">
-        <v>24</v>
-      </c>
-      <c r="D6" s="11">
-        <f t="shared" ref="D6:D16" si="2">(((A6*B6)/256)*50*C6)/(10^6)</f>
-        <v>9.7200000000000006</v>
-      </c>
-      <c r="E6" s="14">
-        <f t="shared" si="0"/>
-        <v>18.339622641509436</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" si="1"/>
-        <v>107.88013318534964</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>1280</v>
-      </c>
-      <c r="B7" s="5">
-        <v>720</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>2.3868</v>
+      </c>
+      <c r="E13" s="18">
+        <f t="shared" si="1"/>
+        <v>4.5033962264150942</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="2"/>
+        <v>26.490566037735849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>416</v>
+      </c>
+      <c r="B14" s="4">
+        <v>240</v>
+      </c>
+      <c r="C14" s="4">
         <v>60</v>
       </c>
-      <c r="D7" s="11">
-        <f t="shared" si="2"/>
-        <v>10.8</v>
-      </c>
-      <c r="E7" s="14">
-        <f t="shared" si="0"/>
-        <v>20.377358490566039</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="1"/>
-        <v>119.86681465038848</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>1280</v>
-      </c>
-      <c r="B8" s="5">
-        <v>720</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1934</v>
+      </c>
+      <c r="E14" s="18">
+        <f t="shared" si="1"/>
+        <v>2.2516981132075471</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="2"/>
+        <v>13.245283018867925</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>416</v>
+      </c>
+      <c r="B15" s="4">
+        <v>240</v>
+      </c>
+      <c r="C15" s="4">
+        <v>50</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99450000000000005</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" si="1"/>
+        <v>1.8764150943396227</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="2"/>
+        <v>11.037735849056604</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>416</v>
+      </c>
+      <c r="B16" s="6">
+        <v>240</v>
+      </c>
+      <c r="C16" s="6">
         <v>30</v>
       </c>
-      <c r="D8" s="11">
-        <f t="shared" si="2"/>
-        <v>5.4</v>
-      </c>
-      <c r="E8" s="14">
-        <f t="shared" si="0"/>
-        <v>10.188679245283019</v>
-      </c>
-      <c r="F8" s="14">
-        <f t="shared" si="1"/>
-        <v>59.933407325194239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>1280</v>
-      </c>
-      <c r="B9" s="5">
-        <v>720</v>
-      </c>
-      <c r="C9" s="6">
-        <v>20</v>
-      </c>
-      <c r="D9" s="11">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="E9" s="14">
-        <f t="shared" si="0"/>
-        <v>6.7924528301886795</v>
-      </c>
-      <c r="F9" s="14">
-        <f t="shared" si="1"/>
-        <v>39.955604883462826</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>1024</v>
-      </c>
-      <c r="B10" s="5">
-        <v>768</v>
-      </c>
-      <c r="C10" s="6">
-        <v>30</v>
-      </c>
-      <c r="D10" s="11">
-        <f t="shared" si="2"/>
-        <v>4.6079999999999997</v>
-      </c>
-      <c r="E10" s="14">
-        <f t="shared" si="0"/>
-        <v>8.6943396226415093</v>
-      </c>
-      <c r="F10" s="14">
-        <f t="shared" si="1"/>
-        <v>51.143174250832409</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>832</v>
-      </c>
-      <c r="B11" s="5">
-        <v>480</v>
-      </c>
-      <c r="C11" s="6">
-        <v>60</v>
-      </c>
-      <c r="D11" s="11">
-        <f t="shared" si="2"/>
-        <v>4.68</v>
-      </c>
-      <c r="E11" s="14">
-        <f t="shared" si="0"/>
-        <v>8.8301886792452819</v>
-      </c>
-      <c r="F11" s="14">
-        <f t="shared" si="1"/>
-        <v>51.942286348501661</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>832</v>
-      </c>
-      <c r="B12" s="5">
-        <v>480</v>
-      </c>
-      <c r="C12" s="6">
-        <v>50</v>
-      </c>
-      <c r="D12" s="11">
-        <f t="shared" si="2"/>
-        <v>3.9</v>
-      </c>
-      <c r="E12" s="14">
-        <f t="shared" si="0"/>
-        <v>7.3584905660377355</v>
-      </c>
-      <c r="F12" s="14">
-        <f t="shared" si="1"/>
-        <v>43.28523862375139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>832</v>
-      </c>
-      <c r="B13" s="5">
-        <v>480</v>
-      </c>
-      <c r="C13" s="6">
-        <v>30</v>
-      </c>
-      <c r="D13" s="11">
-        <f t="shared" si="2"/>
-        <v>2.34</v>
-      </c>
-      <c r="E13" s="14">
-        <f t="shared" si="0"/>
-        <v>4.415094339622641</v>
-      </c>
-      <c r="F13" s="14">
-        <f t="shared" si="1"/>
-        <v>25.97114317425083</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>416</v>
-      </c>
-      <c r="B14" s="5">
-        <v>240</v>
-      </c>
-      <c r="C14" s="6">
-        <v>60</v>
-      </c>
-      <c r="D14" s="11">
-        <f t="shared" si="2"/>
-        <v>1.17</v>
-      </c>
-      <c r="E14" s="14">
-        <f t="shared" si="0"/>
-        <v>2.2075471698113205</v>
-      </c>
-      <c r="F14" s="14">
-        <f t="shared" si="1"/>
-        <v>12.985571587125415</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>416</v>
-      </c>
-      <c r="B15" s="5">
-        <v>240</v>
-      </c>
-      <c r="C15" s="6">
-        <v>50</v>
-      </c>
-      <c r="D15" s="11">
-        <f t="shared" si="2"/>
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="E15" s="14">
-        <f t="shared" si="0"/>
-        <v>1.8396226415094339</v>
-      </c>
-      <c r="F15" s="14">
-        <f t="shared" si="1"/>
-        <v>10.821309655937847</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>416</v>
-      </c>
-      <c r="B16" s="8">
-        <v>240</v>
-      </c>
-      <c r="C16" s="9">
-        <v>30</v>
-      </c>
-      <c r="D16" s="12">
-        <f t="shared" si="2"/>
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="E16" s="15">
-        <f t="shared" si="0"/>
-        <v>1.1037735849056602</v>
-      </c>
-      <c r="F16" s="15">
-        <f t="shared" si="1"/>
-        <v>6.4927857935627076</v>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.59670000000000001</v>
+      </c>
+      <c r="E16" s="19">
+        <f t="shared" si="1"/>
+        <v>1.1258490566037735</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" si="2"/>
+        <v>6.6226415094339623</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
@@ -1031,11 +1018,11 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ora provo ad aumentare la percentuale di utilizzo
In seguito al colloquio del 29-04 col prof, ci siamo resi conto che ci sono blocchi
di complessita' anche elevata che hanno una percentuale di utilizzo molto bassa, come
ad esempio i barrel shifter. A questo punto creo un branch in cui cerco di ottimizzare
questi blocchi, anche eventualmente a discapito della latenza. Me lo posso permettere
perche', secondo le mie stime, ho ancora diversi cicli di clock a disposizione prima di toccare
la soglia dei 500MHz imposta dalle tecnologie tipiche.
</commit_message>
<xml_diff>
--- a/timing-diagram/timing_analysis_data.xlsx
+++ b/timing-diagram/timing_analysis_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AME_Block-Diagram\timing-diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E461E440-6C35-4BFE-A5A1-62A90A56D76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AF566C-FC57-40AA-9019-5E3B0CBDE0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B0B85157-5F58-4FAA-AB16-990C0694D044}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>w</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Usage Percentage (64x64)</t>
+  </si>
+  <si>
+    <t>Carchiamo di aumentare la percentuale di utilizzo senza sfondare i 500MHz</t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -565,6 +574,20 @@
     <xf numFmtId="2" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -883,7 +906,7 @@
   <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +918,8 @@
     <col min="8" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="13" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -948,7 +972,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="7">
-        <f>(((A2*B2)/256)*$N$11*C2)/(10^6)</f>
+        <f t="shared" ref="D2:D16" si="0">(((A2*B2)/256)*$N$11*C2)/(10^6)</f>
         <v>24.48</v>
       </c>
       <c r="E2" s="20">
@@ -956,11 +980,11 @@
         <v>46.188679245283019</v>
       </c>
       <c r="F2" s="42">
-        <f>E2*(100/$N$8)</f>
+        <f t="shared" ref="F2:F16" si="1">E2*(100/$N$8)</f>
         <v>271.69811320754718</v>
       </c>
       <c r="G2" s="7">
-        <f>(((A2*B2)/1024)*$N$13*C2)/(10^6)</f>
+        <f t="shared" ref="G2:G16" si="2">(((A2*B2)/1024)*$N$13*C2)/(10^6)</f>
         <v>17.16</v>
       </c>
       <c r="H2" s="7">
@@ -968,11 +992,11 @@
         <v>32.377358490566039</v>
       </c>
       <c r="I2" s="46">
-        <f>H2*(100/$N$8)</f>
+        <f t="shared" ref="I2:I16" si="3">H2*(100/$N$8)</f>
         <v>190.45504994450613</v>
       </c>
       <c r="J2" s="7">
-        <f>(((A2*B2)/4096)*$N$15*C2)/(10^6)</f>
+        <f t="shared" ref="J2:J16" si="4">(((A2*B2)/4096)*$N$15*C2)/(10^6)</f>
         <v>15.81</v>
       </c>
       <c r="K2" s="7">
@@ -980,7 +1004,7 @@
         <v>29.830188679245285</v>
       </c>
       <c r="L2" s="49">
-        <f>K2*(100/$N$8)</f>
+        <f t="shared" ref="L2:L16" si="5">K2*(100/$N$8)</f>
         <v>175.47169811320757</v>
       </c>
       <c r="M2" s="53"/>
@@ -996,39 +1020,39 @@
         <v>60</v>
       </c>
       <c r="D3" s="8">
-        <f>(((A3*B3)/256)*$N$11*C3)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>24.786000000000001</v>
       </c>
       <c r="E3" s="22">
-        <f t="shared" ref="E3:E16" si="0">D3*(100/$N$6)</f>
+        <f t="shared" ref="E3:E16" si="6">D3*(100/$N$6)</f>
         <v>46.766037735849061</v>
       </c>
       <c r="F3" s="43">
-        <f>E3*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>275.09433962264154</v>
       </c>
       <c r="G3" s="8">
-        <f>(((A3*B3)/1024)*$N$13*C3)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>17.374500000000001</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" ref="H3:H16" si="1">G3*(100/$N$6)</f>
+        <f t="shared" ref="H3:H16" si="7">G3*(100/$N$6)</f>
         <v>32.782075471698114</v>
       </c>
       <c r="I3" s="47">
-        <f>H3*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>192.83573806881245</v>
       </c>
       <c r="J3" s="8">
-        <f>(((A3*B3)/4096)*$N$15*C3)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>16.007625000000001</v>
       </c>
       <c r="K3" s="8">
-        <f t="shared" ref="K3:K16" si="2">J3*(100/$N$6)</f>
+        <f t="shared" ref="K3:K16" si="8">J3*(100/$N$6)</f>
         <v>30.203066037735852</v>
       </c>
       <c r="L3" s="50">
-        <f>K3*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>177.66509433962267</v>
       </c>
       <c r="M3" s="53"/>
@@ -1044,39 +1068,39 @@
         <v>50</v>
       </c>
       <c r="D4" s="8">
-        <f>(((A4*B4)/256)*$N$11*C4)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>20.655000000000001</v>
       </c>
       <c r="E4" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>38.971698113207552</v>
       </c>
       <c r="F4" s="43">
-        <f>E4*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>229.24528301886798</v>
       </c>
       <c r="G4" s="8">
-        <f>(((A4*B4)/1024)*$N$13*C4)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>14.47875</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>27.318396226415093</v>
       </c>
       <c r="I4" s="47">
-        <f>H4*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>160.69644839067703</v>
       </c>
       <c r="J4" s="8">
-        <f>(((A4*B4)/4096)*$N$15*C4)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>13.3396875</v>
       </c>
       <c r="K4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>25.169221698113208</v>
       </c>
       <c r="L4" s="50">
-        <f>K4*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>148.05424528301887</v>
       </c>
       <c r="M4" s="53"/>
@@ -1092,39 +1116,39 @@
         <v>30</v>
       </c>
       <c r="D5" s="8">
-        <f>(((A5*B5)/256)*$N$11*C5)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>12.393000000000001</v>
       </c>
       <c r="E5" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>23.38301886792453</v>
       </c>
       <c r="F5" s="43">
-        <f>E5*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>137.54716981132077</v>
       </c>
       <c r="G5" s="8">
-        <f>(((A5*B5)/1024)*$N$13*C5)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>8.6872500000000006</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>16.391037735849057</v>
       </c>
       <c r="I5" s="47">
-        <f>H5*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>96.417869034406223</v>
       </c>
       <c r="J5" s="8">
-        <f>(((A5*B5)/4096)*$N$15*C5)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>8.0038125000000004</v>
       </c>
       <c r="K5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>15.101533018867926</v>
       </c>
       <c r="L5" s="50">
-        <f>K5*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>88.832547169811335</v>
       </c>
       <c r="M5" s="53"/>
@@ -1143,39 +1167,39 @@
         <v>24</v>
       </c>
       <c r="D6" s="8">
-        <f>(((A6*B6)/256)*$N$11*C6)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>9.9144000000000005</v>
       </c>
       <c r="E6" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>18.706415094339626</v>
       </c>
       <c r="F6" s="43">
-        <f>E6*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>110.03773584905663</v>
       </c>
       <c r="G6" s="8">
-        <f>(((A6*B6)/1024)*$N$13*C6)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>6.9497999999999998</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>13.112830188679245</v>
       </c>
       <c r="I6" s="47">
-        <f>H6*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>77.134295227524973</v>
       </c>
       <c r="J6" s="8">
-        <f>(((A6*B6)/4096)*$N$15*C6)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>6.4030500000000004</v>
       </c>
       <c r="K6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>12.08122641509434</v>
       </c>
       <c r="L6" s="50">
-        <f>K6*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>71.066037735849065</v>
       </c>
       <c r="M6" s="53"/>
@@ -1197,39 +1221,39 @@
         <v>60</v>
       </c>
       <c r="D7" s="8">
-        <f>(((A7*B7)/256)*$N$11*C7)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>11.016</v>
       </c>
       <c r="E7" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>20.784905660377358</v>
       </c>
       <c r="F7" s="43">
-        <f>E7*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>122.26415094339623</v>
       </c>
       <c r="G7" s="8">
-        <f>(((A7*B7)/1024)*$N$13*C7)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>7.7220000000000004</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>14.569811320754718</v>
       </c>
       <c r="I7" s="47">
-        <f>H7*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>85.704772475027767</v>
       </c>
       <c r="J7" s="8">
-        <f>(((A7*B7)/4096)*$N$15*C7)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>7.1144999999999996</v>
       </c>
       <c r="K7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>13.423584905660377</v>
       </c>
       <c r="L7" s="50">
-        <f>K7*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>78.962264150943398</v>
       </c>
       <c r="M7" s="53"/>
@@ -1248,39 +1272,39 @@
         <v>30</v>
       </c>
       <c r="D8" s="8">
-        <f>(((A8*B8)/256)*$N$11*C8)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>5.508</v>
       </c>
       <c r="E8" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>10.392452830188679</v>
       </c>
       <c r="F8" s="43">
-        <f>E8*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>61.132075471698116</v>
       </c>
       <c r="G8" s="8">
-        <f>(((A8*B8)/1024)*$N$13*C8)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>3.8610000000000002</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>7.2849056603773592</v>
       </c>
       <c r="I8" s="47">
-        <f>H8*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>42.852386237513883</v>
       </c>
       <c r="J8" s="8">
-        <f>(((A8*B8)/4096)*$N$15*C8)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>3.5572499999999998</v>
       </c>
       <c r="K8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6.7117924528301884</v>
       </c>
       <c r="L8" s="50">
-        <f>K8*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>39.481132075471699</v>
       </c>
       <c r="M8" s="53"/>
@@ -1302,39 +1326,39 @@
         <v>20</v>
       </c>
       <c r="D9" s="8">
-        <f>(((A9*B9)/256)*$N$11*C9)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>3.6720000000000002</v>
       </c>
       <c r="E9" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>6.9283018867924531</v>
       </c>
       <c r="F9" s="43">
-        <f>E9*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>40.754716981132077</v>
       </c>
       <c r="G9" s="8">
-        <f>(((A9*B9)/1024)*$N$13*C9)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>2.5739999999999998</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>4.8566037735849052</v>
       </c>
       <c r="I9" s="47">
-        <f>H9*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>28.568257491675915</v>
       </c>
       <c r="J9" s="8">
-        <f>(((A9*B9)/4096)*$N$15*C9)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>2.3715000000000002</v>
       </c>
       <c r="K9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.4745283018867932</v>
       </c>
       <c r="L9" s="50">
-        <f>K9*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>26.320754716981138</v>
       </c>
       <c r="M9" s="53"/>
@@ -1350,39 +1374,39 @@
         <v>30</v>
       </c>
       <c r="D10" s="8">
-        <f>(((A10*B10)/256)*$N$11*C10)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>4.7001600000000003</v>
       </c>
       <c r="E10" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>8.8682264150943411</v>
       </c>
       <c r="F10" s="43">
-        <f>E10*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>52.166037735849066</v>
       </c>
       <c r="G10" s="8">
-        <f>(((A10*B10)/1024)*$N$13*C10)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>3.2947199999999999</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>6.216452830188679</v>
       </c>
       <c r="I10" s="47">
-        <f>H10*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>36.567369589345176</v>
       </c>
       <c r="J10" s="8">
-        <f>(((A10*B10)/4096)*$N$15*C10)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>3.03552</v>
       </c>
       <c r="K10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.7273962264150944</v>
       </c>
       <c r="L10" s="50">
-        <f>K10*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>33.690566037735849</v>
       </c>
       <c r="M10" s="53"/>
@@ -1405,39 +1429,39 @@
         <v>60</v>
       </c>
       <c r="D11" s="8">
-        <f>(((A11*B11)/256)*$N$11*C11)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>4.7736000000000001</v>
       </c>
       <c r="E11" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>9.0067924528301884</v>
       </c>
       <c r="F11" s="43">
-        <f>E11*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>52.981132075471699</v>
       </c>
       <c r="G11" s="8">
-        <f>(((A11*B11)/1024)*$N$13*C11)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>3.3462000000000001</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>6.3135849056603774</v>
       </c>
       <c r="I11" s="47">
-        <f>H11*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>37.138734739178695</v>
       </c>
       <c r="J11" s="8">
-        <f>(((A11*B11)/4096)*$N$15*C11)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>3.0829499999999999</v>
       </c>
       <c r="K11" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.8168867924528298</v>
       </c>
       <c r="L11" s="50">
-        <f>K11*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>34.216981132075475</v>
       </c>
       <c r="M11" s="53"/>
@@ -1456,39 +1480,39 @@
         <v>50</v>
       </c>
       <c r="D12" s="8">
-        <f>(((A12*B12)/256)*$N$11*C12)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>3.9780000000000002</v>
       </c>
       <c r="E12" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>7.5056603773584909</v>
       </c>
       <c r="F12" s="43">
-        <f>E12*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>44.150943396226417</v>
       </c>
       <c r="G12" s="8">
-        <f>(((A12*B12)/1024)*$N$13*C12)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>2.7885</v>
       </c>
       <c r="H12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>5.2613207547169809</v>
       </c>
       <c r="I12" s="47">
-        <f>H12*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>30.948945615982243</v>
       </c>
       <c r="J12" s="8">
-        <f>(((A12*B12)/4096)*$N$15*C12)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>2.5691250000000001</v>
       </c>
       <c r="K12" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.8474056603773583</v>
       </c>
       <c r="L12" s="50">
-        <f>K12*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>28.514150943396228</v>
       </c>
       <c r="M12" s="53"/>
@@ -1511,39 +1535,39 @@
         <v>30</v>
       </c>
       <c r="D13" s="8">
-        <f>(((A13*B13)/256)*$N$11*C13)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>2.3868</v>
       </c>
       <c r="E13" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>4.5033962264150942</v>
       </c>
       <c r="F13" s="43">
-        <f>E13*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>26.490566037735849</v>
       </c>
       <c r="G13" s="8">
-        <f>(((A13*B13)/1024)*$N$13*C13)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>1.6731</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>3.1567924528301887</v>
       </c>
       <c r="I13" s="47">
-        <f>H13*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>18.569367369589347</v>
       </c>
       <c r="J13" s="8">
-        <f>(((A13*B13)/4096)*$N$15*C13)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>1.5414749999999999</v>
       </c>
       <c r="K13" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.9084433962264149</v>
       </c>
       <c r="L13" s="50">
-        <f>K13*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>17.108490566037737</v>
       </c>
       <c r="M13" s="53"/>
@@ -1562,39 +1586,39 @@
         <v>60</v>
       </c>
       <c r="D14" s="8">
-        <f>(((A14*B14)/256)*$N$11*C14)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>1.1934</v>
       </c>
       <c r="E14" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>2.2516981132075471</v>
       </c>
       <c r="F14" s="43">
-        <f>E14*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>13.245283018867925</v>
       </c>
       <c r="G14" s="8">
-        <f>(((A14*B14)/1024)*$N$13*C14)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>0.83655000000000002</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.5783962264150944</v>
       </c>
       <c r="I14" s="47">
-        <f>H14*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>9.2846836847946737</v>
       </c>
       <c r="J14" s="8">
-        <f>(((A14*B14)/4096)*$N$15*C14)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>0.77073749999999996</v>
       </c>
       <c r="K14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.4542216981132075</v>
       </c>
       <c r="L14" s="50">
-        <f>K14*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>8.5542452830188687</v>
       </c>
       <c r="M14" s="53"/>
@@ -1617,39 +1641,39 @@
         <v>50</v>
       </c>
       <c r="D15" s="8">
-        <f>(((A15*B15)/256)*$N$11*C15)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>0.99450000000000005</v>
       </c>
       <c r="E15" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>1.8764150943396227</v>
       </c>
       <c r="F15" s="43">
-        <f>E15*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>11.037735849056604</v>
       </c>
       <c r="G15" s="8">
-        <f>(((A15*B15)/1024)*$N$13*C15)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>0.69712499999999999</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.3153301886792452</v>
       </c>
       <c r="I15" s="47">
-        <f>H15*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>7.7372364039955608</v>
       </c>
       <c r="J15" s="8">
-        <f>(((A15*B15)/4096)*$N$15*C15)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>0.64228125000000003</v>
       </c>
       <c r="K15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.2118514150943396</v>
       </c>
       <c r="L15" s="50">
-        <f>K15*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>7.1285377358490569</v>
       </c>
       <c r="M15" s="53"/>
@@ -1668,39 +1692,39 @@
         <v>30</v>
       </c>
       <c r="D16" s="9">
-        <f>(((A16*B16)/256)*$N$11*C16)/(10^6)</f>
+        <f t="shared" si="0"/>
         <v>0.59670000000000001</v>
       </c>
       <c r="E16" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>1.1258490566037735</v>
       </c>
       <c r="F16" s="44">
-        <f>E16*(100/$N$8)</f>
+        <f t="shared" si="1"/>
         <v>6.6226415094339623</v>
       </c>
       <c r="G16" s="9">
-        <f>(((A16*B16)/1024)*$N$13*C16)/(10^6)</f>
+        <f t="shared" si="2"/>
         <v>0.41827500000000001</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.78919811320754718</v>
       </c>
       <c r="I16" s="48">
-        <f>H16*(100/$N$8)</f>
+        <f t="shared" si="3"/>
         <v>4.6423418423973368</v>
       </c>
       <c r="J16" s="9">
-        <f>(((A16*B16)/4096)*$N$15*C16)/(10^6)</f>
+        <f t="shared" si="4"/>
         <v>0.38536874999999998</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.72711084905660373</v>
       </c>
       <c r="L16" s="51">
-        <f>K16*(100/$N$8)</f>
+        <f t="shared" si="5"/>
         <v>4.2771226415094343</v>
       </c>
       <c r="M16" s="53"/>
@@ -1908,7 +1932,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6:V32"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,7 +2209,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10:P15"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,105 +2320,108 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="55">
         <v>2</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="56">
         <v>2</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="55">
         <f>D4</f>
         <v>2</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="57">
         <f>D4</f>
         <v>2</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="58">
         <f t="shared" si="0"/>
         <v>3.9215686274509802</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="59">
         <f t="shared" si="1"/>
         <v>1.3986013986013985</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="60">
         <f t="shared" si="2"/>
         <v>0.37950664136622392</v>
       </c>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="62">
         <v>4</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="63">
         <f>4*2</f>
         <v>8</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="62">
         <f>D5*4</f>
         <v>32</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="64">
         <f>D5*16</f>
         <v>128</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="65">
         <f t="shared" si="0"/>
         <v>15.686274509803921</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="66">
         <f t="shared" si="1"/>
         <v>22.377622377622377</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="67">
         <f t="shared" si="2"/>
         <v>24.288425047438331</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="55">
         <v>2</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="56">
         <f>D5</f>
         <v>8</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="55">
         <f>E5</f>
         <v>32</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="57">
         <f>F5</f>
         <v>128</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="58">
         <f t="shared" si="0"/>
         <v>15.686274509803921</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="59">
         <f t="shared" si="1"/>
         <v>22.377622377622377</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="60">
         <f t="shared" si="2"/>
         <v>24.288425047438331</v>
       </c>

</xml_diff>

<commit_message>
Number of clock cycles corrected
</commit_message>
<xml_diff>
--- a/timing-diagram/timing_analysis_data.xlsx
+++ b/timing-diagram/timing_analysis_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AME_Block-Diagram\timing-diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AF566C-FC57-40AA-9019-5E3B0CBDE0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6150E5F7-9C08-4CDB-892F-9F66484B0C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B0B85157-5F58-4FAA-AB16-990C0694D044}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>w</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Latenza post-memoria (scelta del best candidate)</t>
-  </si>
-  <si>
-    <t>scrittura nel rf di uscita</t>
   </si>
   <si>
     <t>Esempio 64x64</t>
@@ -903,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBD2D36-072C-4FA3-BFF3-6C9E50610318}">
-  <dimension ref="A1:R76"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,39 +970,39 @@
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:D16" si="0">(((A2*B2)/256)*$N$11*C2)/(10^6)</f>
-        <v>24.48</v>
+        <v>24</v>
       </c>
       <c r="E2" s="20">
         <f>D2*(100/$N$6)</f>
-        <v>46.188679245283019</v>
+        <v>45.283018867924525</v>
       </c>
       <c r="F2" s="42">
         <f t="shared" ref="F2:F16" si="1">E2*(100/$N$8)</f>
-        <v>271.69811320754718</v>
+        <v>266.37069922308547</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" ref="G2:G16" si="2">(((A2*B2)/1024)*$N$13*C2)/(10^6)</f>
-        <v>17.16</v>
+        <v>17.04</v>
       </c>
       <c r="H2" s="7">
         <f>G2*(100/$N$6)</f>
-        <v>32.377358490566039</v>
+        <v>32.150943396226417</v>
       </c>
       <c r="I2" s="46">
         <f t="shared" ref="I2:I16" si="3">H2*(100/$N$8)</f>
-        <v>190.45504994450613</v>
+        <v>189.1231964483907</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" ref="J2:J16" si="4">(((A2*B2)/4096)*$N$15*C2)/(10^6)</f>
-        <v>15.81</v>
+        <v>15.78</v>
       </c>
       <c r="K2" s="7">
         <f>J2*(100/$N$6)</f>
-        <v>29.830188679245285</v>
+        <v>29.773584905660378</v>
       </c>
       <c r="L2" s="49">
         <f t="shared" ref="L2:L16" si="5">K2*(100/$N$8)</f>
-        <v>175.47169811320757</v>
+        <v>175.13873473917872</v>
       </c>
       <c r="M2" s="53"/>
     </row>
@@ -1021,39 +1018,39 @@
       </c>
       <c r="D3" s="8">
         <f t="shared" si="0"/>
-        <v>24.786000000000001</v>
+        <v>24.3</v>
       </c>
       <c r="E3" s="22">
         <f t="shared" ref="E3:E16" si="6">D3*(100/$N$6)</f>
-        <v>46.766037735849061</v>
+        <v>45.84905660377359</v>
       </c>
       <c r="F3" s="43">
         <f t="shared" si="1"/>
-        <v>275.09433962264154</v>
+        <v>269.70033296337408</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" si="2"/>
-        <v>17.374500000000001</v>
+        <v>17.253</v>
       </c>
       <c r="H3" s="8">
         <f t="shared" ref="H3:H16" si="7">G3*(100/$N$6)</f>
-        <v>32.782075471698114</v>
+        <v>32.552830188679245</v>
       </c>
       <c r="I3" s="47">
         <f t="shared" si="3"/>
-        <v>192.83573806881245</v>
+        <v>191.48723640399558</v>
       </c>
       <c r="J3" s="8">
         <f t="shared" si="4"/>
-        <v>16.007625000000001</v>
+        <v>15.97725</v>
       </c>
       <c r="K3" s="8">
         <f t="shared" ref="K3:K16" si="8">J3*(100/$N$6)</f>
-        <v>30.203066037735852</v>
+        <v>30.145754716981131</v>
       </c>
       <c r="L3" s="50">
         <f t="shared" si="5"/>
-        <v>177.66509433962267</v>
+        <v>177.32796892341844</v>
       </c>
       <c r="M3" s="53"/>
     </row>
@@ -1069,39 +1066,39 @@
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
-        <v>20.655000000000001</v>
+        <v>20.25</v>
       </c>
       <c r="E4" s="22">
         <f t="shared" si="6"/>
-        <v>38.971698113207552</v>
+        <v>38.20754716981132</v>
       </c>
       <c r="F4" s="43">
         <f t="shared" si="1"/>
-        <v>229.24528301886798</v>
+        <v>224.75027746947836</v>
       </c>
       <c r="G4" s="8">
         <f t="shared" si="2"/>
-        <v>14.47875</v>
+        <v>14.3775</v>
       </c>
       <c r="H4" s="8">
         <f t="shared" si="7"/>
-        <v>27.318396226415093</v>
+        <v>27.127358490566039</v>
       </c>
       <c r="I4" s="47">
         <f t="shared" si="3"/>
-        <v>160.69644839067703</v>
+        <v>159.57269700332964</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" si="4"/>
-        <v>13.3396875</v>
+        <v>13.314375</v>
       </c>
       <c r="K4" s="8">
         <f t="shared" si="8"/>
-        <v>25.169221698113208</v>
+        <v>25.121462264150942</v>
       </c>
       <c r="L4" s="50">
         <f t="shared" si="5"/>
-        <v>148.05424528301887</v>
+        <v>147.77330743618202</v>
       </c>
       <c r="M4" s="53"/>
     </row>
@@ -1117,39 +1114,39 @@
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
-        <v>12.393000000000001</v>
+        <v>12.15</v>
       </c>
       <c r="E5" s="22">
         <f t="shared" si="6"/>
-        <v>23.38301886792453</v>
+        <v>22.924528301886795</v>
       </c>
       <c r="F5" s="43">
         <f t="shared" si="1"/>
-        <v>137.54716981132077</v>
+        <v>134.85016648168704</v>
       </c>
       <c r="G5" s="8">
         <f t="shared" si="2"/>
-        <v>8.6872500000000006</v>
+        <v>8.6265000000000001</v>
       </c>
       <c r="H5" s="8">
         <f t="shared" si="7"/>
-        <v>16.391037735849057</v>
+        <v>16.276415094339622</v>
       </c>
       <c r="I5" s="47">
         <f t="shared" si="3"/>
-        <v>96.417869034406223</v>
+        <v>95.743618201997791</v>
       </c>
       <c r="J5" s="8">
         <f t="shared" si="4"/>
-        <v>8.0038125000000004</v>
+        <v>7.9886249999999999</v>
       </c>
       <c r="K5" s="8">
         <f t="shared" si="8"/>
-        <v>15.101533018867926</v>
+        <v>15.072877358490565</v>
       </c>
       <c r="L5" s="50">
         <f t="shared" si="5"/>
-        <v>88.832547169811335</v>
+        <v>88.663984461709219</v>
       </c>
       <c r="M5" s="53"/>
       <c r="N5" t="s">
@@ -1168,39 +1165,39 @@
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>9.9144000000000005</v>
+        <v>9.7200000000000006</v>
       </c>
       <c r="E6" s="22">
         <f t="shared" si="6"/>
-        <v>18.706415094339626</v>
+        <v>18.339622641509436</v>
       </c>
       <c r="F6" s="43">
         <f t="shared" si="1"/>
-        <v>110.03773584905663</v>
+        <v>107.88013318534964</v>
       </c>
       <c r="G6" s="8">
         <f t="shared" si="2"/>
-        <v>6.9497999999999998</v>
+        <v>6.9012000000000002</v>
       </c>
       <c r="H6" s="8">
         <f t="shared" si="7"/>
-        <v>13.112830188679245</v>
+        <v>13.021132075471698</v>
       </c>
       <c r="I6" s="47">
         <f t="shared" si="3"/>
-        <v>77.134295227524973</v>
+        <v>76.594894561598224</v>
       </c>
       <c r="J6" s="8">
         <f t="shared" si="4"/>
-        <v>6.4030500000000004</v>
+        <v>6.3909000000000002</v>
       </c>
       <c r="K6" s="8">
         <f t="shared" si="8"/>
-        <v>12.08122641509434</v>
+        <v>12.058301886792453</v>
       </c>
       <c r="L6" s="50">
         <f t="shared" si="5"/>
-        <v>71.066037735849065</v>
+        <v>70.931187569367381</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6">
@@ -1222,39 +1219,39 @@
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
-        <v>11.016</v>
+        <v>10.8</v>
       </c>
       <c r="E7" s="22">
         <f t="shared" si="6"/>
-        <v>20.784905660377358</v>
+        <v>20.377358490566039</v>
       </c>
       <c r="F7" s="43">
         <f t="shared" si="1"/>
-        <v>122.26415094339623</v>
+        <v>119.86681465038848</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" si="2"/>
-        <v>7.7220000000000004</v>
+        <v>7.6680000000000001</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="7"/>
-        <v>14.569811320754718</v>
+        <v>14.467924528301888</v>
       </c>
       <c r="I7" s="47">
         <f t="shared" si="3"/>
-        <v>85.704772475027767</v>
+        <v>85.105438401775814</v>
       </c>
       <c r="J7" s="8">
         <f t="shared" si="4"/>
-        <v>7.1144999999999996</v>
+        <v>7.101</v>
       </c>
       <c r="K7" s="8">
         <f t="shared" si="8"/>
-        <v>13.423584905660377</v>
+        <v>13.398113207547169</v>
       </c>
       <c r="L7" s="50">
         <f t="shared" si="5"/>
-        <v>78.962264150943398</v>
+        <v>78.812430632630409</v>
       </c>
       <c r="M7" s="53"/>
       <c r="N7" t="s">
@@ -1273,39 +1270,39 @@
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
-        <v>5.508</v>
+        <v>5.4</v>
       </c>
       <c r="E8" s="22">
         <f t="shared" si="6"/>
-        <v>10.392452830188679</v>
+        <v>10.188679245283019</v>
       </c>
       <c r="F8" s="43">
         <f t="shared" si="1"/>
-        <v>61.132075471698116</v>
+        <v>59.933407325194239</v>
       </c>
       <c r="G8" s="8">
         <f t="shared" si="2"/>
-        <v>3.8610000000000002</v>
+        <v>3.8340000000000001</v>
       </c>
       <c r="H8" s="8">
         <f t="shared" si="7"/>
-        <v>7.2849056603773592</v>
+        <v>7.2339622641509438</v>
       </c>
       <c r="I8" s="47">
         <f t="shared" si="3"/>
-        <v>42.852386237513883</v>
+        <v>42.552719200887907</v>
       </c>
       <c r="J8" s="8">
         <f t="shared" si="4"/>
-        <v>3.5572499999999998</v>
+        <v>3.5505</v>
       </c>
       <c r="K8" s="8">
         <f t="shared" si="8"/>
-        <v>6.7117924528301884</v>
+        <v>6.6990566037735846</v>
       </c>
       <c r="L8" s="50">
         <f t="shared" si="5"/>
-        <v>39.481132075471699</v>
+        <v>39.406215316315205</v>
       </c>
       <c r="M8" s="53"/>
       <c r="N8">
@@ -1327,39 +1324,39 @@
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
-        <v>3.6720000000000002</v>
+        <v>3.6</v>
       </c>
       <c r="E9" s="22">
         <f t="shared" si="6"/>
-        <v>6.9283018867924531</v>
+        <v>6.7924528301886795</v>
       </c>
       <c r="F9" s="43">
         <f t="shared" si="1"/>
-        <v>40.754716981132077</v>
+        <v>39.955604883462826</v>
       </c>
       <c r="G9" s="8">
         <f t="shared" si="2"/>
-        <v>2.5739999999999998</v>
+        <v>2.556</v>
       </c>
       <c r="H9" s="8">
         <f t="shared" si="7"/>
-        <v>4.8566037735849052</v>
+        <v>4.8226415094339625</v>
       </c>
       <c r="I9" s="47">
         <f t="shared" si="3"/>
-        <v>28.568257491675915</v>
+        <v>28.368479467258606</v>
       </c>
       <c r="J9" s="8">
         <f t="shared" si="4"/>
-        <v>2.3715000000000002</v>
+        <v>2.367</v>
       </c>
       <c r="K9" s="8">
         <f t="shared" si="8"/>
-        <v>4.4745283018867932</v>
+        <v>4.4660377358490564</v>
       </c>
       <c r="L9" s="50">
         <f t="shared" si="5"/>
-        <v>26.320754716981138</v>
+        <v>26.270810210876803</v>
       </c>
       <c r="M9" s="53"/>
     </row>
@@ -1375,43 +1372,43 @@
       </c>
       <c r="D10" s="8">
         <f t="shared" si="0"/>
-        <v>4.7001600000000003</v>
+        <v>4.6079999999999997</v>
       </c>
       <c r="E10" s="22">
         <f t="shared" si="6"/>
-        <v>8.8682264150943411</v>
+        <v>8.6943396226415093</v>
       </c>
       <c r="F10" s="43">
         <f t="shared" si="1"/>
-        <v>52.166037735849066</v>
+        <v>51.143174250832409</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="2"/>
-        <v>3.2947199999999999</v>
+        <v>3.2716799999999999</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="7"/>
-        <v>6.216452830188679</v>
+        <v>6.1729811320754715</v>
       </c>
       <c r="I10" s="47">
         <f t="shared" si="3"/>
-        <v>36.567369589345176</v>
+        <v>36.311653718091009</v>
       </c>
       <c r="J10" s="8">
         <f t="shared" si="4"/>
-        <v>3.03552</v>
+        <v>3.02976</v>
       </c>
       <c r="K10" s="8">
         <f t="shared" si="8"/>
-        <v>5.7273962264150944</v>
+        <v>5.7165283018867923</v>
       </c>
       <c r="L10" s="50">
         <f t="shared" si="5"/>
-        <v>33.690566037735849</v>
+        <v>33.62663706992231</v>
       </c>
       <c r="M10" s="53"/>
       <c r="N10" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
@@ -1430,43 +1427,44 @@
       </c>
       <c r="D11" s="8">
         <f t="shared" si="0"/>
-        <v>4.7736000000000001</v>
+        <v>4.68</v>
       </c>
       <c r="E11" s="22">
         <f t="shared" si="6"/>
-        <v>9.0067924528301884</v>
+        <v>8.8301886792452819</v>
       </c>
       <c r="F11" s="43">
         <f t="shared" si="1"/>
-        <v>52.981132075471699</v>
+        <v>51.942286348501661</v>
       </c>
       <c r="G11" s="8">
         <f t="shared" si="2"/>
-        <v>3.3462000000000001</v>
+        <v>3.3228</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" si="7"/>
-        <v>6.3135849056603774</v>
+        <v>6.2694339622641513</v>
       </c>
       <c r="I11" s="47">
         <f t="shared" si="3"/>
-        <v>37.138734739178695</v>
+        <v>36.879023307436185</v>
       </c>
       <c r="J11" s="8">
         <f t="shared" si="4"/>
-        <v>3.0829499999999999</v>
+        <v>3.0771000000000002</v>
       </c>
       <c r="K11" s="8">
         <f t="shared" si="8"/>
-        <v>5.8168867924528298</v>
+        <v>5.8058490566037744</v>
       </c>
       <c r="L11" s="50">
         <f t="shared" si="5"/>
-        <v>34.216981132075475</v>
+        <v>34.152053274139853</v>
       </c>
       <c r="M11" s="53"/>
       <c r="N11">
-        <v>51</v>
+        <f>A56</f>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1481,43 +1479,43 @@
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
-        <v>3.9780000000000002</v>
+        <v>3.9</v>
       </c>
       <c r="E12" s="22">
         <f t="shared" si="6"/>
-        <v>7.5056603773584909</v>
+        <v>7.3584905660377355</v>
       </c>
       <c r="F12" s="43">
         <f t="shared" si="1"/>
-        <v>44.150943396226417</v>
+        <v>43.28523862375139</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" si="2"/>
-        <v>2.7885</v>
+        <v>2.7690000000000001</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="7"/>
-        <v>5.2613207547169809</v>
+        <v>5.2245283018867932</v>
       </c>
       <c r="I12" s="47">
         <f t="shared" si="3"/>
-        <v>30.948945615982243</v>
+        <v>30.73251942286349</v>
       </c>
       <c r="J12" s="8">
         <f t="shared" si="4"/>
-        <v>2.5691250000000001</v>
+        <v>2.5642499999999999</v>
       </c>
       <c r="K12" s="8">
         <f t="shared" si="8"/>
-        <v>4.8474056603773583</v>
+        <v>4.8382075471698114</v>
       </c>
       <c r="L12" s="50">
         <f t="shared" si="5"/>
-        <v>28.514150943396228</v>
+        <v>28.46004439511654</v>
       </c>
       <c r="M12" s="53"/>
       <c r="N12" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O12" s="15"/>
       <c r="P12" s="15"/>
@@ -1536,43 +1534,44 @@
       </c>
       <c r="D13" s="8">
         <f t="shared" si="0"/>
-        <v>2.3868</v>
+        <v>2.34</v>
       </c>
       <c r="E13" s="22">
         <f t="shared" si="6"/>
-        <v>4.5033962264150942</v>
+        <v>4.415094339622641</v>
       </c>
       <c r="F13" s="43">
         <f t="shared" si="1"/>
-        <v>26.490566037735849</v>
+        <v>25.97114317425083</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" si="2"/>
-        <v>1.6731</v>
+        <v>1.6614</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="7"/>
-        <v>3.1567924528301887</v>
+        <v>3.1347169811320756</v>
       </c>
       <c r="I13" s="47">
         <f t="shared" si="3"/>
-        <v>18.569367369589347</v>
+        <v>18.439511653718093</v>
       </c>
       <c r="J13" s="8">
         <f t="shared" si="4"/>
-        <v>1.5414749999999999</v>
+        <v>1.5385500000000001</v>
       </c>
       <c r="K13" s="8">
         <f t="shared" si="8"/>
-        <v>2.9084433962264149</v>
+        <v>2.9029245283018872</v>
       </c>
       <c r="L13" s="50">
         <f t="shared" si="5"/>
-        <v>17.108490566037737</v>
+        <v>17.076026637069926</v>
       </c>
       <c r="M13" s="53"/>
       <c r="N13">
-        <v>143</v>
+        <f>A64</f>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1587,39 +1586,39 @@
       </c>
       <c r="D14" s="8">
         <f t="shared" si="0"/>
-        <v>1.1934</v>
+        <v>1.17</v>
       </c>
       <c r="E14" s="22">
         <f t="shared" si="6"/>
-        <v>2.2516981132075471</v>
+        <v>2.2075471698113205</v>
       </c>
       <c r="F14" s="43">
         <f t="shared" si="1"/>
-        <v>13.245283018867925</v>
+        <v>12.985571587125415</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" si="2"/>
-        <v>0.83655000000000002</v>
+        <v>0.83069999999999999</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="7"/>
-        <v>1.5783962264150944</v>
+        <v>1.5673584905660378</v>
       </c>
       <c r="I14" s="47">
         <f t="shared" si="3"/>
-        <v>9.2846836847946737</v>
+        <v>9.2197558268590463</v>
       </c>
       <c r="J14" s="8">
         <f t="shared" si="4"/>
-        <v>0.77073749999999996</v>
+        <v>0.76927500000000004</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" si="8"/>
-        <v>1.4542216981132075</v>
+        <v>1.4514622641509436</v>
       </c>
       <c r="L14" s="50">
         <f t="shared" si="5"/>
-        <v>8.5542452830188687</v>
+        <v>8.5380133185349631</v>
       </c>
       <c r="M14" s="53"/>
       <c r="N14" s="16" t="s">
@@ -1642,43 +1641,44 @@
       </c>
       <c r="D15" s="8">
         <f t="shared" si="0"/>
-        <v>0.99450000000000005</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E15" s="22">
         <f t="shared" si="6"/>
-        <v>1.8764150943396227</v>
+        <v>1.8396226415094339</v>
       </c>
       <c r="F15" s="43">
         <f t="shared" si="1"/>
-        <v>11.037735849056604</v>
+        <v>10.821309655937847</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="2"/>
-        <v>0.69712499999999999</v>
+        <v>0.69225000000000003</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="7"/>
-        <v>1.3153301886792452</v>
+        <v>1.3061320754716983</v>
       </c>
       <c r="I15" s="47">
         <f t="shared" si="3"/>
-        <v>7.7372364039955608</v>
+        <v>7.6831298557158725</v>
       </c>
       <c r="J15" s="8">
         <f t="shared" si="4"/>
-        <v>0.64228125000000003</v>
+        <v>0.64106249999999998</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" si="8"/>
-        <v>1.2118514150943396</v>
+        <v>1.2095518867924528</v>
       </c>
       <c r="L15" s="50">
         <f t="shared" si="5"/>
-        <v>7.1285377358490569</v>
+        <v>7.1150110987791351</v>
       </c>
       <c r="M15" s="53"/>
       <c r="N15">
-        <v>527</v>
+        <f>A72</f>
+        <v>526</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1693,39 +1693,39 @@
       </c>
       <c r="D16" s="9">
         <f t="shared" si="0"/>
-        <v>0.59670000000000001</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="E16" s="24">
         <f t="shared" si="6"/>
-        <v>1.1258490566037735</v>
+        <v>1.1037735849056602</v>
       </c>
       <c r="F16" s="44">
         <f t="shared" si="1"/>
-        <v>6.6226415094339623</v>
+        <v>6.4927857935627076</v>
       </c>
       <c r="G16" s="9">
         <f t="shared" si="2"/>
-        <v>0.41827500000000001</v>
+        <v>0.41535</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="7"/>
-        <v>0.78919811320754718</v>
+        <v>0.78367924528301891</v>
       </c>
       <c r="I16" s="48">
         <f t="shared" si="3"/>
-        <v>4.6423418423973368</v>
+        <v>4.6098779134295231</v>
       </c>
       <c r="J16" s="9">
         <f t="shared" si="4"/>
-        <v>0.38536874999999998</v>
+        <v>0.38463750000000002</v>
       </c>
       <c r="K16" s="9">
         <f t="shared" si="8"/>
-        <v>0.72711084905660373</v>
+        <v>0.7257311320754718</v>
       </c>
       <c r="L16" s="51">
         <f t="shared" si="5"/>
-        <v>4.2771226415094343</v>
+        <v>4.2690066592674816</v>
       </c>
       <c r="M16" s="53"/>
     </row>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B55" t="s">
         <v>20</v>
@@ -1792,134 +1792,110 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>2</v>
-      </c>
-      <c r="B56" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <f>SUM(A51:A56)</f>
-        <v>51</v>
+        <f>SUM(A51:A55)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>22</v>
+      <c r="A60">
+        <v>64</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>256</v>
-      </c>
-      <c r="B64" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>5</v>
-      </c>
-      <c r="B65" t="s">
-        <v>20</v>
+        <f>SUM(A59:A63)</f>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>2</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="A66" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f>SUM(A61:A66)</f>
-        <v>527</v>
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>256</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>40</v>
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>0</v>
-      </c>
-      <c r="B72" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>64</v>
-      </c>
-      <c r="B73" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>5</v>
-      </c>
-      <c r="B74" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>2</v>
-      </c>
-      <c r="B75" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <f>SUM(A70:A75)</f>
-        <v>143</v>
+        <f>SUM(A67:A71)</f>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -1929,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C87860-CAD2-47BF-803D-1910712C592E}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,152 +1927,152 @@
         <v>14</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="38" t="s">
         <v>70</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="27">
         <v>12</v>
       </c>
       <c r="E2" s="8">
         <f>D2/$J$11*100</f>
-        <v>23.52941176470588</v>
+        <v>24</v>
       </c>
       <c r="F2" s="8">
         <f>E2/$J$13*100</f>
-        <v>16.454134101192924</v>
+        <v>16.901408450704224</v>
       </c>
       <c r="G2" s="39">
         <f t="shared" ref="G2:G8" si="0">D2/$J$15*100</f>
-        <v>2.2770398481973433</v>
+        <v>2.2813688212927756</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4">
         <v>6</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="27">
         <v>12</v>
       </c>
       <c r="E3" s="8">
         <f t="shared" ref="E3:E8" si="1">D3/$J$11*100</f>
-        <v>23.52941176470588</v>
+        <v>24</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F8" si="2">E3/$J$13*100</f>
-        <v>16.454134101192924</v>
+        <v>16.901408450704224</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" si="0"/>
-        <v>2.2770398481973433</v>
+        <v>2.2813688212927756</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="27">
         <v>1</v>
       </c>
       <c r="E4" s="8">
         <f t="shared" si="1"/>
-        <v>1.9607843137254901</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8">
         <f t="shared" si="2"/>
-        <v>1.3711778417660769</v>
+        <v>1.4084507042253522</v>
       </c>
       <c r="G4" s="39">
         <f t="shared" si="0"/>
-        <v>0.18975332068311196</v>
+        <v>0.19011406844106463</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="26">
         <v>12</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="1"/>
-        <v>23.52941176470588</v>
+        <v>24</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="2"/>
-        <v>16.454134101192924</v>
+        <v>16.901408450704224</v>
       </c>
       <c r="G5" s="41">
         <f t="shared" si="0"/>
-        <v>2.2770398481973433</v>
+        <v>2.2813688212927756</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="27">
         <v>12</v>
       </c>
       <c r="E6" s="8">
         <f t="shared" si="1"/>
-        <v>23.52941176470588</v>
+        <v>24</v>
       </c>
       <c r="F6" s="8">
         <f t="shared" si="2"/>
-        <v>16.454134101192924</v>
+        <v>16.901408450704224</v>
       </c>
       <c r="G6" s="39">
         <f t="shared" si="0"/>
-        <v>2.2770398481973433</v>
+        <v>2.2813688212927756</v>
       </c>
       <c r="J6" t="s">
         <v>13</v>
@@ -2104,28 +2080,28 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="27">
         <v>12</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="1"/>
-        <v>23.52941176470588</v>
+        <v>24</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="2"/>
-        <v>16.454134101192924</v>
+        <v>16.901408450704224</v>
       </c>
       <c r="G7" s="39">
         <f t="shared" si="0"/>
-        <v>2.2770398481973433</v>
+        <v>2.2813688212927756</v>
       </c>
       <c r="J7">
         <v>21</v>
@@ -2133,33 +2109,33 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6">
         <v>2</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="28">
         <v>12</v>
       </c>
       <c r="E8" s="9">
         <f t="shared" si="1"/>
-        <v>23.52941176470588</v>
+        <v>24</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="2"/>
-        <v>16.454134101192924</v>
+        <v>16.901408450704224</v>
       </c>
       <c r="G8" s="40">
         <f t="shared" si="0"/>
-        <v>2.2770398481973433</v>
+        <v>2.2813688212927756</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J10" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -2168,12 +2144,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J11">
-        <v>51</v>
+        <f>A56</f>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J12" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -2182,7 +2159,8 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J13">
-        <v>143</v>
+        <f>A64</f>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2196,7 +2174,161 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J15">
-        <v>527</v>
+        <f>A72</f>
+        <v>526</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>16</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f>SUM(A51:A55)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>64</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>64</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f>SUM(A59:A63)</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>256</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>256</v>
+      </c>
+      <c r="B70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f>SUM(A67:A71)</f>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -2209,7 +2341,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2227,39 +2359,39 @@
         <v>14</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="29">
         <v>3</v>
@@ -2274,26 +2406,26 @@
       </c>
       <c r="G2" s="20">
         <f>D2/$L$11*100</f>
-        <v>5.8823529411764701</v>
+        <v>6</v>
       </c>
       <c r="H2" s="7">
         <f>E2/$L$13*100</f>
-        <v>2.0979020979020979</v>
+        <v>2.112676056338028</v>
       </c>
       <c r="I2" s="21">
         <f>F2/$L$15*100</f>
-        <v>0.56925996204933582</v>
+        <v>0.57034220532319391</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="30">
         <v>2</v>
@@ -2308,26 +2440,26 @@
       </c>
       <c r="G3" s="22">
         <f t="shared" ref="G3:G16" si="0">D3/$L$11*100</f>
-        <v>3.9215686274509802</v>
+        <v>4</v>
       </c>
       <c r="H3" s="8">
         <f t="shared" ref="H3:H16" si="1">E3/$L$13*100</f>
-        <v>1.3986013986013985</v>
+        <v>1.4084507042253522</v>
       </c>
       <c r="I3" s="23">
         <f t="shared" ref="I3:I16" si="2">F3/$L$15*100</f>
-        <v>0.37950664136622392</v>
+        <v>0.38022813688212925</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="55">
         <v>2</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="56">
         <v>2</v>
@@ -2342,29 +2474,29 @@
       </c>
       <c r="G4" s="58">
         <f t="shared" si="0"/>
-        <v>3.9215686274509802</v>
+        <v>4</v>
       </c>
       <c r="H4" s="59">
         <f t="shared" si="1"/>
-        <v>1.3986013986013985</v>
+        <v>1.4084507042253522</v>
       </c>
       <c r="I4" s="60">
         <f t="shared" si="2"/>
-        <v>0.37950664136622392</v>
+        <v>0.38022813688212925</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="62">
         <v>4</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="63">
         <f>4*2</f>
@@ -2380,26 +2512,26 @@
       </c>
       <c r="G5" s="65">
         <f t="shared" si="0"/>
-        <v>15.686274509803921</v>
+        <v>16</v>
       </c>
       <c r="H5" s="66">
         <f t="shared" si="1"/>
-        <v>22.377622377622377</v>
+        <v>22.535211267605636</v>
       </c>
       <c r="I5" s="67">
         <f t="shared" si="2"/>
-        <v>24.288425047438331</v>
+        <v>24.334600760456272</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="55">
         <v>2</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="56">
         <f>D5</f>
@@ -2415,26 +2547,26 @@
       </c>
       <c r="G6" s="58">
         <f t="shared" si="0"/>
-        <v>15.686274509803921</v>
+        <v>16</v>
       </c>
       <c r="H6" s="59">
         <f t="shared" si="1"/>
-        <v>22.377622377622377</v>
+        <v>22.535211267605636</v>
       </c>
       <c r="I6" s="60">
         <f t="shared" si="2"/>
-        <v>24.288425047438331</v>
+        <v>24.334600760456272</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="30">
         <f>D5</f>
@@ -2450,26 +2582,26 @@
       </c>
       <c r="G7" s="22">
         <f t="shared" si="0"/>
-        <v>15.686274509803921</v>
+        <v>16</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="1"/>
-        <v>22.377622377622377</v>
+        <v>22.535211267605636</v>
       </c>
       <c r="I7" s="23">
         <f t="shared" si="2"/>
-        <v>24.288425047438331</v>
+        <v>24.334600760456272</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="31">
         <f>D5</f>
@@ -2485,26 +2617,26 @@
       </c>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>15.686274509803921</v>
+        <v>16</v>
       </c>
       <c r="H8" s="9">
         <f t="shared" si="1"/>
-        <v>22.377622377622377</v>
+        <v>22.535211267605636</v>
       </c>
       <c r="I8" s="25">
         <f t="shared" si="2"/>
-        <v>24.288425047438331</v>
+        <v>24.334600760456272</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="29">
         <f>16*2</f>
@@ -2520,26 +2652,26 @@
       </c>
       <c r="G9" s="20">
         <f t="shared" si="0"/>
-        <v>62.745098039215684</v>
+        <v>64</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>89.510489510489506</v>
+        <v>90.140845070422543</v>
       </c>
       <c r="I9" s="21">
         <f t="shared" si="2"/>
-        <v>97.153700189753323</v>
+        <v>97.338403041825089</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="30">
         <f t="shared" ref="D10:F11" si="3">D9</f>
@@ -2555,18 +2687,18 @@
       </c>
       <c r="G10" s="22">
         <f t="shared" si="0"/>
-        <v>62.745098039215684</v>
+        <v>64</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="1"/>
-        <v>89.510489510489506</v>
+        <v>90.140845070422543</v>
       </c>
       <c r="I10" s="23">
         <f t="shared" si="2"/>
-        <v>97.153700189753323</v>
+        <v>97.338403041825089</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
@@ -2575,13 +2707,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="4">
         <v>4</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="30">
         <f t="shared" si="3"/>
@@ -2597,29 +2729,29 @@
       </c>
       <c r="G11" s="22">
         <f t="shared" si="0"/>
-        <v>62.745098039215684</v>
+        <v>64</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" si="1"/>
-        <v>89.510489510489506</v>
+        <v>90.140845070422543</v>
       </c>
       <c r="I11" s="23">
         <f t="shared" si="2"/>
-        <v>97.153700189753323</v>
+        <v>97.338403041825089</v>
       </c>
       <c r="L11">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="30">
         <f>D9</f>
@@ -2635,18 +2767,18 @@
       </c>
       <c r="G12" s="22">
         <f t="shared" si="0"/>
-        <v>62.745098039215684</v>
+        <v>64</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="1"/>
-        <v>89.510489510489506</v>
+        <v>90.140845070422543</v>
       </c>
       <c r="I12" s="23">
         <f t="shared" si="2"/>
-        <v>97.153700189753323</v>
+        <v>97.338403041825089</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -2655,13 +2787,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="30">
         <f>D9</f>
@@ -2677,29 +2809,29 @@
       </c>
       <c r="G13" s="22">
         <f t="shared" si="0"/>
-        <v>62.745098039215684</v>
+        <v>64</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="1"/>
-        <v>89.510489510489506</v>
+        <v>90.140845070422543</v>
       </c>
       <c r="I13" s="23">
         <f t="shared" si="2"/>
-        <v>97.153700189753323</v>
+        <v>97.338403041825089</v>
       </c>
       <c r="L13">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="31">
         <f>D9</f>
@@ -2715,15 +2847,15 @@
       </c>
       <c r="G14" s="24">
         <f t="shared" si="0"/>
-        <v>62.745098039215684</v>
+        <v>64</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="1"/>
-        <v>89.510489510489506</v>
+        <v>90.140845070422543</v>
       </c>
       <c r="I14" s="25">
         <f t="shared" si="2"/>
-        <v>97.153700189753323</v>
+        <v>97.338403041825089</v>
       </c>
       <c r="L14" s="16" t="s">
         <v>15</v>
@@ -2735,13 +2867,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="30">
         <v>2</v>
@@ -2754,29 +2886,29 @@
       </c>
       <c r="G15" s="22">
         <f t="shared" si="0"/>
-        <v>3.9215686274509802</v>
+        <v>4</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="1"/>
-        <v>1.3986013986013985</v>
+        <v>1.4084507042253522</v>
       </c>
       <c r="I15" s="23">
         <f t="shared" si="2"/>
-        <v>0.37950664136622392</v>
+        <v>0.38022813688212925</v>
       </c>
       <c r="L15">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="6">
         <v>1</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="31">
         <v>1</v>
@@ -2789,15 +2921,15 @@
       </c>
       <c r="G16" s="24">
         <f t="shared" si="0"/>
-        <v>1.9607843137254901</v>
+        <v>2</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="1"/>
-        <v>0.69930069930069927</v>
+        <v>0.70422535211267612</v>
       </c>
       <c r="I16" s="25">
         <f t="shared" si="2"/>
-        <v>0.18975332068311196</v>
+        <v>0.19011406844106463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>